<commit_message>
First cut of show and hide bug functional test
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v11_RDM-4687_hideandshow_complextype.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v11_RDM-4687_hideandshow_complextype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/Documents/Definition Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedanaskhatri/project/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B9C73FB-D813-2545-BC08-C1AC17A21B1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA83F01-6789-7F49-BF08-048656D020E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="541">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1723,6 +1723,30 @@
   </si>
   <si>
     <t>AddressHidden</t>
+  </si>
+  <si>
+    <t>SecondAddress</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>Country="US"</t>
+  </si>
+  <si>
+    <t>Second Line 1</t>
+  </si>
+  <si>
+    <t>Second Line 2</t>
+  </si>
+  <si>
+    <t>SecondLine1</t>
+  </si>
+  <si>
+    <t>SecondLine2</t>
+  </si>
+  <si>
+    <t>SecondLine1="1"</t>
   </si>
 </sst>
 </file>
@@ -3765,8 +3789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView showGridLines="0" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11244,7 +11268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
@@ -21645,10 +21669,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21796,17 +21820,17 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="8" t="s">
-        <v>51</v>
+        <v>533</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>99</v>
+        <v>538</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="8" t="s">
-        <v>100</v>
+        <v>536</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7"/>
@@ -21828,19 +21852,21 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="8" t="s">
-        <v>51</v>
+        <v>533</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>101</v>
+        <v>539</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="8"/>
+        <v>537</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>540</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
@@ -21863,14 +21889,14 @@
         <v>51</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="7"/>
@@ -21895,14 +21921,14 @@
         <v>51</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="7"/>
@@ -21924,17 +21950,17 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="8" t="s">
-        <v>532</v>
+        <v>51</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="7"/>
@@ -21956,17 +21982,17 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="8" t="s">
-        <v>532</v>
+        <v>51</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="7"/>
@@ -21988,19 +22014,21 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="8" t="s">
-        <v>532</v>
+        <v>51</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>103</v>
+        <v>534</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" s="8"/>
+        <v>534</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>535</v>
+      </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="8" t="s">
@@ -22020,17 +22048,17 @@
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="8" t="s">
-        <v>532</v>
+        <v>51</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>105</v>
+        <v>533</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>48</v>
+        <v>533</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
-        <v>105</v>
+        <v>533</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="7"/>
@@ -22046,73 +22074,69 @@
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" s="183" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="184">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="184"/>
+    <row r="12" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="10"/>
       <c r="C12" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="D12" s="185" t="s">
-        <v>526</v>
-      </c>
-      <c r="E12" s="185" t="s">
+      <c r="D12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="187"/>
-      <c r="G12" s="185" t="s">
-        <v>527</v>
-      </c>
-      <c r="H12" s="185" t="s">
-        <v>528</v>
-      </c>
-      <c r="I12" s="187"/>
-      <c r="J12" s="187"/>
-      <c r="K12" s="185" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="187"/>
-      <c r="M12" s="187"/>
-      <c r="N12" s="187"/>
-      <c r="O12" s="187"/>
-      <c r="P12" s="187"/>
-      <c r="Q12" s="187"/>
-      <c r="R12" s="187"/>
-    </row>
-    <row r="13" spans="1:18" s="183" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="184">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="184"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="10"/>
       <c r="C13" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="D13" s="185" t="s">
-        <v>529</v>
-      </c>
-      <c r="E13" s="185" t="s">
+      <c r="D13" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="187"/>
-      <c r="G13" s="185" t="s">
-        <v>530</v>
-      </c>
-      <c r="H13" s="185" t="s">
-        <v>531</v>
-      </c>
-      <c r="I13" s="187"/>
-      <c r="J13" s="187"/>
-      <c r="K13" s="185" t="s">
+      <c r="F13" s="7"/>
+      <c r="G13" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="187"/>
-      <c r="M13" s="187"/>
-      <c r="N13" s="187"/>
-      <c r="O13" s="187"/>
-      <c r="P13" s="187"/>
-      <c r="Q13" s="187"/>
-      <c r="R13" s="187"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
@@ -22120,17 +22144,17 @@
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="8" t="s">
-        <v>65</v>
+        <v>532</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="7"/>
@@ -22146,69 +22170,73 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="10"/>
+    <row r="15" spans="1:18" s="183" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="184">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="184"/>
       <c r="C15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="D15" s="185" t="s">
+        <v>526</v>
+      </c>
+      <c r="E15" s="185" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-    </row>
-    <row r="16" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="10"/>
+      <c r="F15" s="187"/>
+      <c r="G15" s="185" t="s">
+        <v>527</v>
+      </c>
+      <c r="H15" s="185" t="s">
+        <v>528</v>
+      </c>
+      <c r="I15" s="187"/>
+      <c r="J15" s="187"/>
+      <c r="K15" s="185" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="187"/>
+      <c r="M15" s="187"/>
+      <c r="N15" s="187"/>
+      <c r="O15" s="187"/>
+      <c r="P15" s="187"/>
+      <c r="Q15" s="187"/>
+      <c r="R15" s="187"/>
+    </row>
+    <row r="16" spans="1:18" s="183" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="184">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="184"/>
       <c r="C16" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="D16" s="185" t="s">
+        <v>529</v>
+      </c>
+      <c r="E16" s="185" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
+      <c r="F16" s="187"/>
+      <c r="G16" s="185" t="s">
+        <v>530</v>
+      </c>
+      <c r="H16" s="185" t="s">
+        <v>531</v>
+      </c>
+      <c r="I16" s="187"/>
+      <c r="J16" s="187"/>
+      <c r="K16" s="185" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="187"/>
+      <c r="M16" s="187"/>
+      <c r="N16" s="187"/>
+      <c r="O16" s="187"/>
+      <c r="P16" s="187"/>
+      <c r="Q16" s="187"/>
+      <c r="R16" s="187"/>
     </row>
     <row r="17" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
@@ -22219,14 +22247,14 @@
         <v>65</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="7"/>
@@ -22251,14 +22279,14 @@
         <v>65</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="7"/>
@@ -22283,14 +22311,14 @@
         <v>65</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="7"/>
@@ -22312,17 +22340,17 @@
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="8" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="7"/>
@@ -22344,23 +22372,23 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="8" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="8" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
@@ -22376,23 +22404,23 @@
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="8" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -22402,29 +22430,29 @@
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
     </row>
-    <row r="23" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
         <v>42736</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="8" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
@@ -22434,29 +22462,29 @@
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
     </row>
-    <row r="24" spans="1:18" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>42736</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
@@ -22466,23 +22494,23 @@
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
     </row>
-    <row r="25" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10">
         <v>42736</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="D25" s="57" t="s">
-        <v>299</v>
+        <v>119</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8" t="s">
-        <v>298</v>
+        <v>12</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="7"/>
@@ -22498,31 +22526,29 @@
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
     </row>
-    <row r="26" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="10">
         <v>42736</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="D26" s="57" t="s">
-        <v>301</v>
+        <v>119</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>304</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>302</v>
+        <v>116</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="8" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -22532,29 +22558,29 @@
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
     </row>
-    <row r="27" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="10">
         <v>42736</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="8" t="s">
-        <v>297</v>
+        <v>119</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>300</v>
+        <v>117</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
-        <v>303</v>
+        <v>118</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
@@ -22564,119 +22590,121 @@
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
     </row>
-    <row r="28" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="104">
-        <v>42736</v>
-      </c>
-      <c r="B28" s="104"/>
-      <c r="C28" s="105" t="s">
+    <row r="28" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="D28" s="106" t="s">
-        <v>428</v>
-      </c>
-      <c r="E28" s="106" t="s">
-        <v>429</v>
-      </c>
-      <c r="F28" s="107"/>
-      <c r="G28" s="106" t="s">
-        <v>430</v>
-      </c>
-      <c r="H28" s="105"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="106" t="s">
+      <c r="D28" s="57" t="s">
+        <v>299</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="H28" s="8"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L28" s="107"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-    </row>
-    <row r="29" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="104">
-        <v>42736</v>
-      </c>
-      <c r="B29" s="104"/>
-      <c r="C29" s="106" t="s">
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+    </row>
+    <row r="29" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="D29" s="106" t="s">
-        <v>461</v>
-      </c>
-      <c r="E29" s="106" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="107"/>
-      <c r="G29" s="106" t="s">
-        <v>446</v>
-      </c>
-      <c r="H29" s="105"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="106" t="s">
+      <c r="D29" s="57" t="s">
+        <v>301</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L29" s="107"/>
-      <c r="M29" s="107"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-    </row>
-    <row r="30" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="104">
-        <v>42736</v>
-      </c>
-      <c r="B30" s="104"/>
-      <c r="C30" s="106" t="s">
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+    </row>
+    <row r="30" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="D30" s="106" t="s">
-        <v>443</v>
-      </c>
-      <c r="E30" s="106" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" s="107"/>
-      <c r="G30" s="106" t="s">
-        <v>444</v>
-      </c>
-      <c r="H30" s="105"/>
-      <c r="I30" s="107"/>
-      <c r="J30" s="107"/>
-      <c r="K30" s="106" t="s">
+      <c r="D30" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L30" s="107"/>
-      <c r="M30" s="107"/>
-      <c r="N30" s="107"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
     </row>
     <row r="31" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="104">
         <v>42736</v>
       </c>
       <c r="B31" s="104"/>
-      <c r="C31" s="106" t="s">
+      <c r="C31" s="105" t="s">
         <v>297</v>
       </c>
       <c r="D31" s="106" t="s">
-        <v>448</v>
+        <v>428</v>
       </c>
       <c r="E31" s="106" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="F31" s="107"/>
       <c r="G31" s="106" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
       <c r="H31" s="105"/>
       <c r="I31" s="107"/>
@@ -22692,103 +22720,103 @@
       <c r="Q31" s="107"/>
       <c r="R31" s="107"/>
     </row>
-    <row r="32" spans="1:18" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="8" t="s">
+    <row r="32" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="104">
+        <v>42736</v>
+      </c>
+      <c r="B32" s="104"/>
+      <c r="C32" s="106" t="s">
+        <v>297</v>
+      </c>
+      <c r="D32" s="106" t="s">
+        <v>461</v>
+      </c>
+      <c r="E32" s="106" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="107"/>
+      <c r="G32" s="106" t="s">
+        <v>446</v>
+      </c>
+      <c r="H32" s="105"/>
+      <c r="I32" s="107"/>
+      <c r="J32" s="107"/>
+      <c r="K32" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-    </row>
-    <row r="33" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="8" t="s">
+      <c r="L32" s="107"/>
+      <c r="M32" s="107"/>
+      <c r="N32" s="107"/>
+      <c r="O32" s="107"/>
+      <c r="P32" s="107"/>
+      <c r="Q32" s="107"/>
+      <c r="R32" s="107"/>
+    </row>
+    <row r="33" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="104">
+        <v>42736</v>
+      </c>
+      <c r="B33" s="104"/>
+      <c r="C33" s="106" t="s">
+        <v>297</v>
+      </c>
+      <c r="D33" s="106" t="s">
+        <v>443</v>
+      </c>
+      <c r="E33" s="106" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="107"/>
+      <c r="G33" s="106" t="s">
+        <v>444</v>
+      </c>
+      <c r="H33" s="105"/>
+      <c r="I33" s="107"/>
+      <c r="J33" s="107"/>
+      <c r="K33" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-    </row>
-    <row r="34" spans="1:18" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="10">
-        <v>42736</v>
-      </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="8" t="s">
+      <c r="L33" s="107"/>
+      <c r="M33" s="107"/>
+      <c r="N33" s="107"/>
+      <c r="O33" s="107"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="107"/>
+      <c r="R33" s="107"/>
+    </row>
+    <row r="34" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="104">
+        <v>42736</v>
+      </c>
+      <c r="B34" s="104"/>
+      <c r="C34" s="106" t="s">
+        <v>297</v>
+      </c>
+      <c r="D34" s="106" t="s">
+        <v>448</v>
+      </c>
+      <c r="E34" s="106" t="s">
+        <v>440</v>
+      </c>
+      <c r="F34" s="107"/>
+      <c r="G34" s="106" t="s">
+        <v>447</v>
+      </c>
+      <c r="H34" s="105"/>
+      <c r="I34" s="107"/>
+      <c r="J34" s="107"/>
+      <c r="K34" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-    </row>
-    <row r="35" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L34" s="107"/>
+      <c r="M34" s="107"/>
+      <c r="N34" s="107"/>
+      <c r="O34" s="107"/>
+      <c r="P34" s="107"/>
+      <c r="Q34" s="107"/>
+      <c r="R34" s="107"/>
+    </row>
+    <row r="35" spans="1:18" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10">
         <v>42736</v>
       </c>
@@ -22797,14 +22825,14 @@
         <v>287</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>48</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="H35" s="8"/>
       <c r="I35" s="7"/>
@@ -22820,25 +22848,23 @@
       <c r="Q35" s="7"/>
       <c r="R35" s="7"/>
     </row>
-    <row r="36" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10">
         <v>42736</v>
       </c>
       <c r="B36" s="10"/>
-      <c r="C36" s="57" t="s">
+      <c r="C36" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="D36" s="57" t="s">
-        <v>296</v>
+      <c r="D36" s="8" t="s">
+        <v>292</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="G36" s="57" t="s">
-        <v>318</v>
+        <v>48</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8" t="s">
+        <v>293</v>
       </c>
       <c r="H36" s="8"/>
       <c r="I36" s="7"/>
@@ -22854,233 +22880,331 @@
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
     </row>
-    <row r="37" spans="1:18" s="161" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="157">
-        <v>42736</v>
-      </c>
-      <c r="B37" s="157"/>
-      <c r="C37" s="165" t="s">
+    <row r="37" spans="1:18" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="D37" s="165" t="s">
+      <c r="D37" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="H37" s="8"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+    </row>
+    <row r="38" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="H38" s="8"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+    </row>
+    <row r="39" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="D39" s="57" t="s">
+        <v>296</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G39" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+    </row>
+    <row r="40" spans="1:18" s="161" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="157">
+        <v>42736</v>
+      </c>
+      <c r="B40" s="157"/>
+      <c r="C40" s="165" t="s">
+        <v>287</v>
+      </c>
+      <c r="D40" s="165" t="s">
         <v>517</v>
       </c>
-      <c r="E37" s="158" t="s">
+      <c r="E40" s="158" t="s">
         <v>429</v>
       </c>
-      <c r="F37" s="159"/>
-      <c r="G37" s="165" t="s">
+      <c r="F40" s="159"/>
+      <c r="G40" s="165" t="s">
         <v>518</v>
       </c>
-      <c r="H37" s="158"/>
-      <c r="I37" s="159"/>
-      <c r="J37" s="159"/>
-      <c r="K37" s="158" t="s">
-        <v>27</v>
-      </c>
-      <c r="L37" s="159"/>
-      <c r="M37" s="159"/>
-      <c r="N37" s="159"/>
-      <c r="O37" s="159"/>
-      <c r="P37" s="159"/>
-      <c r="Q37" s="159"/>
-      <c r="R37" s="159"/>
-    </row>
-    <row r="38" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="104">
-        <v>42736</v>
-      </c>
-      <c r="B38" s="104"/>
-      <c r="C38" s="106" t="s">
-        <v>435</v>
-      </c>
-      <c r="D38" s="106" t="s">
-        <v>432</v>
-      </c>
-      <c r="E38" s="105" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="108"/>
-      <c r="G38" s="106" t="s">
-        <v>433</v>
-      </c>
-      <c r="H38" s="105"/>
-      <c r="I38" s="107"/>
-      <c r="J38" s="107"/>
-      <c r="K38" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="L38" s="107"/>
-      <c r="M38" s="107"/>
-      <c r="N38" s="107"/>
-      <c r="O38" s="107"/>
-      <c r="P38" s="107"/>
-      <c r="Q38" s="107"/>
-      <c r="R38" s="107"/>
-    </row>
-    <row r="39" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="104">
-        <v>42736</v>
-      </c>
-      <c r="B39" s="104"/>
-      <c r="C39" s="106" t="s">
-        <v>435</v>
-      </c>
-      <c r="D39" s="106" t="s">
-        <v>438</v>
-      </c>
-      <c r="E39" s="105" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" s="108" t="s">
-        <v>287</v>
-      </c>
-      <c r="G39" s="106" t="s">
-        <v>441</v>
-      </c>
-      <c r="H39" s="105"/>
-      <c r="I39" s="107"/>
-      <c r="J39" s="107"/>
-      <c r="K39" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="L39" s="107"/>
-      <c r="M39" s="107"/>
-      <c r="N39" s="107"/>
-      <c r="O39" s="107"/>
-      <c r="P39" s="107"/>
-      <c r="Q39" s="107"/>
-      <c r="R39" s="107"/>
-    </row>
-    <row r="40" spans="1:18" s="161" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="157">
-        <v>42736</v>
-      </c>
-      <c r="B40" s="157"/>
-      <c r="C40" s="171" t="s">
-        <v>431</v>
-      </c>
-      <c r="D40" s="172" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="172" t="s">
-        <v>56</v>
-      </c>
-      <c r="F40" s="157"/>
-      <c r="G40" s="172" t="s">
-        <v>519</v>
-      </c>
-      <c r="H40" s="157"/>
-      <c r="I40" s="157"/>
-      <c r="J40" s="157"/>
+      <c r="H40" s="158"/>
+      <c r="I40" s="159"/>
+      <c r="J40" s="159"/>
       <c r="K40" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="L40" s="157"/>
-      <c r="M40" s="157"/>
-      <c r="N40" s="157"/>
-      <c r="O40" s="157"/>
-      <c r="P40" s="157"/>
-      <c r="Q40" s="157"/>
-      <c r="R40" s="157"/>
-    </row>
-    <row r="41" spans="1:18" s="102" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L40" s="159"/>
+      <c r="M40" s="159"/>
+      <c r="N40" s="159"/>
+      <c r="O40" s="159"/>
+      <c r="P40" s="159"/>
+      <c r="Q40" s="159"/>
+      <c r="R40" s="159"/>
+    </row>
+    <row r="41" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="104">
         <v>42736</v>
       </c>
       <c r="B41" s="104"/>
-      <c r="C41" s="109" t="s">
-        <v>431</v>
-      </c>
-      <c r="D41" s="110" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="110" t="s">
+      <c r="C41" s="106" t="s">
+        <v>435</v>
+      </c>
+      <c r="D41" s="106" t="s">
+        <v>432</v>
+      </c>
+      <c r="E41" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="104"/>
-      <c r="G41" s="110" t="s">
-        <v>449</v>
-      </c>
-      <c r="H41" s="104"/>
-      <c r="I41" s="104"/>
-      <c r="J41" s="104"/>
+      <c r="F41" s="108"/>
+      <c r="G41" s="106" t="s">
+        <v>433</v>
+      </c>
+      <c r="H41" s="105"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="107"/>
       <c r="K41" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="L41" s="104"/>
-      <c r="M41" s="104"/>
-      <c r="N41" s="104"/>
-      <c r="O41" s="104"/>
-      <c r="P41" s="104"/>
-      <c r="Q41" s="104"/>
-      <c r="R41" s="104"/>
-    </row>
-    <row r="42" spans="1:18" s="102" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L41" s="107"/>
+      <c r="M41" s="107"/>
+      <c r="N41" s="107"/>
+      <c r="O41" s="107"/>
+      <c r="P41" s="107"/>
+      <c r="Q41" s="107"/>
+      <c r="R41" s="107"/>
+    </row>
+    <row r="42" spans="1:18" s="102" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="104">
         <v>42736</v>
       </c>
       <c r="B42" s="104"/>
-      <c r="C42" s="110" t="s">
+      <c r="C42" s="106" t="s">
+        <v>435</v>
+      </c>
+      <c r="D42" s="106" t="s">
+        <v>438</v>
+      </c>
+      <c r="E42" s="105" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="108" t="s">
+        <v>287</v>
+      </c>
+      <c r="G42" s="106" t="s">
+        <v>441</v>
+      </c>
+      <c r="H42" s="105"/>
+      <c r="I42" s="107"/>
+      <c r="J42" s="107"/>
+      <c r="K42" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="L42" s="107"/>
+      <c r="M42" s="107"/>
+      <c r="N42" s="107"/>
+      <c r="O42" s="107"/>
+      <c r="P42" s="107"/>
+      <c r="Q42" s="107"/>
+      <c r="R42" s="107"/>
+    </row>
+    <row r="43" spans="1:18" s="161" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="157">
+        <v>42736</v>
+      </c>
+      <c r="B43" s="157"/>
+      <c r="C43" s="171" t="s">
         <v>431</v>
       </c>
-      <c r="D42" s="110" t="s">
+      <c r="D43" s="172" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="172" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="157"/>
+      <c r="G43" s="172" t="s">
+        <v>519</v>
+      </c>
+      <c r="H43" s="157"/>
+      <c r="I43" s="157"/>
+      <c r="J43" s="157"/>
+      <c r="K43" s="158" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43" s="157"/>
+      <c r="M43" s="157"/>
+      <c r="N43" s="157"/>
+      <c r="O43" s="157"/>
+      <c r="P43" s="157"/>
+      <c r="Q43" s="157"/>
+      <c r="R43" s="157"/>
+    </row>
+    <row r="44" spans="1:18" s="102" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="104">
+        <v>42736</v>
+      </c>
+      <c r="B44" s="104"/>
+      <c r="C44" s="109" t="s">
+        <v>431</v>
+      </c>
+      <c r="D44" s="110" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="110" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" s="104"/>
+      <c r="G44" s="110" t="s">
+        <v>449</v>
+      </c>
+      <c r="H44" s="104"/>
+      <c r="I44" s="104"/>
+      <c r="J44" s="104"/>
+      <c r="K44" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="L44" s="104"/>
+      <c r="M44" s="104"/>
+      <c r="N44" s="104"/>
+      <c r="O44" s="104"/>
+      <c r="P44" s="104"/>
+      <c r="Q44" s="104"/>
+      <c r="R44" s="104"/>
+    </row>
+    <row r="45" spans="1:18" s="102" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="104">
+        <v>42736</v>
+      </c>
+      <c r="B45" s="104"/>
+      <c r="C45" s="110" t="s">
+        <v>431</v>
+      </c>
+      <c r="D45" s="110" t="s">
         <v>445</v>
       </c>
-      <c r="E42" s="110" t="s">
+      <c r="E45" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="F42" s="104"/>
-      <c r="G42" s="110" t="s">
+      <c r="F45" s="104"/>
+      <c r="G45" s="110" t="s">
         <v>450</v>
       </c>
-      <c r="H42" s="104"/>
-      <c r="I42" s="104"/>
-      <c r="J42" s="104"/>
-      <c r="K42" s="110" t="s">
+      <c r="H45" s="104"/>
+      <c r="I45" s="104"/>
+      <c r="J45" s="104"/>
+      <c r="K45" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="L42" s="98"/>
-      <c r="M42" s="98"/>
-      <c r="N42" s="98"/>
-      <c r="O42" s="98"/>
-      <c r="P42" s="98"/>
-      <c r="Q42" s="98"/>
-      <c r="R42" s="98"/>
-    </row>
-    <row r="43" spans="1:18" s="102" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="104">
-        <v>42736</v>
-      </c>
-      <c r="B43" s="104"/>
-      <c r="C43" s="110" t="s">
+      <c r="L45" s="98"/>
+      <c r="M45" s="98"/>
+      <c r="N45" s="98"/>
+      <c r="O45" s="98"/>
+      <c r="P45" s="98"/>
+      <c r="Q45" s="98"/>
+      <c r="R45" s="98"/>
+    </row>
+    <row r="46" spans="1:18" s="102" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="104">
+        <v>42736</v>
+      </c>
+      <c r="B46" s="104"/>
+      <c r="C46" s="110" t="s">
         <v>431</v>
       </c>
-      <c r="D43" s="110" t="s">
+      <c r="D46" s="110" t="s">
         <v>434</v>
       </c>
-      <c r="E43" s="105" t="s">
+      <c r="E46" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="104" t="s">
+      <c r="F46" s="104" t="s">
         <v>435</v>
       </c>
-      <c r="G43" s="110" t="s">
+      <c r="G46" s="110" t="s">
         <v>451</v>
       </c>
-      <c r="H43" s="104"/>
-      <c r="I43" s="104"/>
-      <c r="J43" s="104"/>
-      <c r="K43" s="110" t="s">
+      <c r="H46" s="104"/>
+      <c r="I46" s="104"/>
+      <c r="J46" s="104"/>
+      <c r="K46" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="L43" s="98"/>
-      <c r="M43" s="98"/>
-      <c r="N43" s="98"/>
-      <c r="O43" s="98"/>
-      <c r="P43" s="98"/>
-      <c r="Q43" s="98"/>
-      <c r="R43" s="98"/>
+      <c r="L46" s="98"/>
+      <c r="M46" s="98"/>
+      <c r="N46" s="98"/>
+      <c r="O46" s="98"/>
+      <c r="P46" s="98"/>
+      <c r="Q46" s="98"/>
+      <c r="R46" s="98"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -23095,7 +23219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E561A8A-480D-6D45-8F14-5D4A9428A511}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -23769,8 +23893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD38"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>